<commit_message>
Updated on 8 Aug 2017
</commit_message>
<xml_diff>
--- a/horizon/xl_templates/48001_DS_CNUS_Ocean.xlsx
+++ b/horizon/xl_templates/48001_DS_CNUS_Ocean.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>Category</t>
+    <t>Vendor</t>
   </si>
   <si>
     <t>From</t>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Trip</t>
-  </si>
-  <si>
-    <t>Vendor</t>
   </si>
 </sst>
 </file>
@@ -389,7 +386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -397,7 +394,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,9 +430,6 @@
       </c>
       <c r="L1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>